<commit_message>
Se agrega un contador para acceder únicamente a los valores de las columnas del archivo excel
</commit_message>
<xml_diff>
--- a/PHPexcel/Materias.xlsx
+++ b/PHPexcel/Materias.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t xml:space="preserve">fullname</t>
   </si>
@@ -176,6 +176,57 @@
   </si>
   <si>
     <t xml:space="preserve">Literatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rubio@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aurora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aurora@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniera industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madelen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">made@outlook.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mecatrónica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vivis@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enfermeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noel@subitus.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teoría de gráficas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marisol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marysol@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -283,13 +334,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.84"/>
@@ -530,6 +581,90 @@
         <v>87989879</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>13648292</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>36474398</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>58477363</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>73887362</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>28376428</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>77384939</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>51</v>
       </c>
     </row>
@@ -551,6 +686,12 @@
     <hyperlink ref="B15" r:id="rId14" display="alberto@gmail.com"/>
     <hyperlink ref="B16" r:id="rId15" display="natalia@outlook.es"/>
     <hyperlink ref="B17" r:id="rId16" display="vianka@subitus.com"/>
+    <hyperlink ref="B18" r:id="rId17" display="rubio@gmail.com"/>
+    <hyperlink ref="B19" r:id="rId18" display="aurora@hotmail.com"/>
+    <hyperlink ref="B20" r:id="rId19" display="made@outlook.es"/>
+    <hyperlink ref="B21" r:id="rId20" display="vivis@gmail.com"/>
+    <hyperlink ref="B22" r:id="rId21" display="noel@subitus.com"/>
+    <hyperlink ref="B23" r:id="rId22" display="marysol@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>